<commit_message>
Finished Complete ER Diagram
Also adjusted my Progress report to reflect hours
</commit_message>
<xml_diff>
--- a/ProgressReports/RyanBury_ProgressReport.xlsx
+++ b/ProgressReports/RyanBury_ProgressReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Design - Revising ER Diagrams and Bidding Section</t>
+  </si>
+  <si>
+    <t>Design - Finished revising ER Diagrams, created complete ER Diagram</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,9 +695,15 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="13">
+        <v>42791</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>

</xml_diff>